<commit_message>
Collapse header icon fix
Making it smaller and fixing event text.
</commit_message>
<xml_diff>
--- a/source/docs/Forplay Objects.xlsx
+++ b/source/docs/Forplay Objects.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Tag</t>
   </si>
@@ -130,6 +133,72 @@
   </si>
   <si>
     <t>object - from the contrusctor argument</t>
+  </si>
+  <si>
+    <t>a.k.a.</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>bg_name</t>
+  </si>
+  <si>
+    <t>en_name</t>
+  </si>
+  <si>
+    <t>main_img</t>
+  </si>
+  <si>
+    <t>smallint(5) unsigned</t>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>AKA</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>aka_name</t>
+  </si>
+  <si>
+    <t>varchar(16)</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>GAMES</t>
+  </si>
+  <si>
+    <t>Гранд Тефт Ауто 5</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto 5</t>
+  </si>
+  <si>
+    <t>gta5.jpg</t>
+  </si>
+  <si>
+    <t>gta-5</t>
+  </si>
+  <si>
+    <t>GTA V</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>ГТА 5</t>
   </si>
 </sst>
 </file>
@@ -200,20 +269,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,9 +620,14 @@
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,211 +646,307 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="6"/>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="H6">
+        <v>65535</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="5" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>65535</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
+      <c r="H16">
+        <v>65535</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -757,10 +955,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -769,7 +967,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -779,7 +977,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -789,7 +987,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -799,7 +997,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -808,8 +1006,8 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>33</v>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -818,8 +1016,8 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
+      <c r="C24" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -828,10 +1026,10 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
@@ -839,10 +1037,10 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,10 +1048,10 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -862,59 +1060,70 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A31:F31"/>
     <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>